<commit_message>
Update to files: script, anexo.
</commit_message>
<xml_diff>
--- a/anexo.xlsx
+++ b/anexo.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\inforcap\bases_de_datos\desafio_ev_1118\github\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\inforcap\bases_de_datos\desafio_ev_1118\github\desafio_1118\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1365DFDD-E361-4175-9878-CBEDA91C77A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74967198-9AE7-42EE-9725-675FCE473BEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{484CCB13-0595-4A7C-9982-1D3CC2C99408}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{484CCB13-0595-4A7C-9982-1D3CC2C99408}"/>
   </bookViews>
   <sheets>
-    <sheet name="REQ6" sheetId="2" r:id="rId1"/>
-    <sheet name="REQ7" sheetId="1" r:id="rId2"/>
+    <sheet name="REQ4" sheetId="3" r:id="rId1"/>
+    <sheet name="REQ6" sheetId="2" r:id="rId2"/>
+    <sheet name="REQ7" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="115">
   <si>
     <t>Forest Gump</t>
   </si>
@@ -338,6 +339,48 @@
   </si>
   <si>
     <t>longitud_titulo</t>
+  </si>
+  <si>
+    <t>Leonardo DiCaprio</t>
+  </si>
+  <si>
+    <t>Kate Winslet</t>
+  </si>
+  <si>
+    <t>Billy Zane</t>
+  </si>
+  <si>
+    <t>Kathy Bates</t>
+  </si>
+  <si>
+    <t>Frances Fisher</t>
+  </si>
+  <si>
+    <t>Bernard Hill</t>
+  </si>
+  <si>
+    <t>Jonathan Hyde</t>
+  </si>
+  <si>
+    <t>Danny Nucci</t>
+  </si>
+  <si>
+    <t>David Warner</t>
+  </si>
+  <si>
+    <t>Bill Paxton</t>
+  </si>
+  <si>
+    <t>Gloria Stuart</t>
+  </si>
+  <si>
+    <t>Victor Garber</t>
+  </si>
+  <si>
+    <t>Suzy Amis</t>
+  </si>
+  <si>
+    <t>actor</t>
   </si>
 </sst>
 </file>
@@ -712,6 +755,94 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{429D8A34-AE0B-411F-B68E-CF0B9CD95359}">
+  <dimension ref="A1:A14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A8BDA69-CE04-498C-A69F-6AF9BE28F4CA}">
   <dimension ref="A1:B31"/>
   <sheetViews>
@@ -884,11 +1015,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02BABFD5-5667-4511-A0AC-6CD05700E737}">
   <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>

</xml_diff>